<commit_message>
Empty Level 6-7 added
</commit_message>
<xml_diff>
--- a/Levels Objectives.xlsx
+++ b/Levels Objectives.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vadim\OneDrive\Desktop\Syntez\Tanchiki\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD481F39-294D-439E-ABE0-F650E84A8946}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D667293-2BDF-4B06-B9E2-31EB51B96BD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -603,8 +603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="97.2" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -745,13 +745,13 @@
         <v>5</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>51</v>
+        <v>5</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>54</v>
+        <v>25</v>
       </c>
       <c r="F5" s="9" t="s">
         <v>41</v>
@@ -774,13 +774,13 @@
         <v>6</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>9</v>
+        <v>52</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>25</v>
+        <v>54</v>
       </c>
       <c r="F6" s="9" t="s">
         <v>40</v>

</xml_diff>

<commit_message>
Work with snow levels
</commit_message>
<xml_diff>
--- a/Levels Objectives.xlsx
+++ b/Levels Objectives.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vadim\OneDrive\Desktop\Syntez\Tanchiki\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D667293-2BDF-4B06-B9E2-31EB51B96BD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE73B030-96F8-44BD-A816-43C80C89EBE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -165,12 +165,6 @@
     <t>Сложный</t>
   </si>
   <si>
-    <t>Большое количество здоровья, имеет две башни: пулеметную, как у раллийного танка и как у Толстяка. Поворотливый, но медленный.</t>
-  </si>
-  <si>
-    <t>Огромное количество здоровья, имеет две башни: пулеметную, как у раллийного танка и как у Толстяка. Поворотливый, но медленный.</t>
-  </si>
-  <si>
     <t>Выглядит как Ratte, размером с толстяка</t>
   </si>
   <si>
@@ -199,6 +193,12 @@
   </si>
   <si>
     <t>Build index</t>
+  </si>
+  <si>
+    <t>Большое количество здоровья. Имеет мощную пушку со средней скорострельностью. Поворотливый, но медленный.</t>
+  </si>
+  <si>
+    <t>Огромное количество здоровья. Имеет мощную пушку со средней скорострельностью. Поворотливый, но медленный.</t>
   </si>
 </sst>
 </file>
@@ -603,8 +603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="97.2" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -623,10 +623,10 @@
   <sheetData>
     <row r="1" spans="1:9" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>55</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>57</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>1</v>
@@ -719,7 +719,7 @@
         <v>8</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>26</v>
@@ -774,13 +774,13 @@
         <v>6</v>
       </c>
       <c r="C6" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>54</v>
       </c>
       <c r="F6" s="9" t="s">
         <v>40</v>
@@ -835,19 +835,19 @@
         <v>34</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F8" s="9" t="s">
         <v>38</v>
       </c>
       <c r="G8" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="H8" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>48</v>
       </c>
       <c r="I8" s="4" t="s">
         <v>45</v>
@@ -858,10 +858,10 @@
         <v>43</v>
       </c>
       <c r="G9" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H9" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>49</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>45</v>

</xml_diff>